<commit_message>
Update script in order to populate db with lots of data
</commit_message>
<xml_diff>
--- a/backend/scripts/data.xlsx
+++ b/backend/scripts/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrians/Desktop/work/devhacks2022/backend/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25854BD7-695B-634C-930A-18F98F0C731E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F53C385-8E17-204B-BCD7-D57925F22E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="2380" windowWidth="28040" windowHeight="17440" xr2:uid="{D3EAF390-8EBA-1D46-B905-68CEE694FD01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>name</t>
   </si>
@@ -120,6 +120,36 @@
   </si>
   <si>
     <t>https://cdn.systematic.com/media/rywmbypl/sse_logo_corpblue_cmyk.png</t>
+  </si>
+  <si>
+    <t>Asociatia Suntem Langa Tine</t>
+  </si>
+  <si>
+    <t>suntemlangatine</t>
+  </si>
+  <si>
+    <t>suntem@gmail.com</t>
+  </si>
+  <si>
+    <t>ong</t>
+  </si>
+  <si>
+    <t>Asociatia Toti pentru Fericire</t>
+  </si>
+  <si>
+    <t>fericiretoti</t>
+  </si>
+  <si>
+    <t>totifericire@gmail.com</t>
+  </si>
+  <si>
+    <t>Green everywhere</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>green@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -482,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E14BE7E-8FEB-B84B-AA20-6499D84EE8B3}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" customWidth="1"/>
     <col min="4" max="4" width="28.1640625" customWidth="1"/>
@@ -634,6 +664,66 @@
       </c>
       <c r="G6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>12345</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>12345</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>12345</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -648,6 +738,9 @@
     <hyperlink ref="D6" r:id="rId8" xr:uid="{24AB44A1-4F37-9740-9BA0-53A81B25C9F2}"/>
     <hyperlink ref="F6" r:id="rId9" xr:uid="{85D17B6B-47EB-BB45-88CF-27A673725E53}"/>
     <hyperlink ref="F5" r:id="rId10" xr:uid="{1C46F769-AB01-2C47-B1C8-547C1D8DE64C}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{48455002-FB18-4043-B02F-05102DD3F5F3}"/>
+    <hyperlink ref="D8" r:id="rId12" xr:uid="{00D9F2BF-AA51-6A47-9C61-2BFE067C7B7F}"/>
+    <hyperlink ref="D9" r:id="rId13" xr:uid="{B16607F2-1D69-6C42-9D19-5B78F7CE8748}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>